<commit_message>
some push i have to do
</commit_message>
<xml_diff>
--- a/Scripts/shot_database_ALL_SHOTS_NewX1X2.xlsx
+++ b/Scripts/shot_database_ALL_SHOTS_NewX1X2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tomas\MAST_Edge_RT_Research\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4490608-F72D-4FAD-BF54-FDA6DED6D95A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A1A14A-87FC-4751-A71A-BB30265B53BA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="201">
   <si>
     <t>shot</t>
   </si>
@@ -494,9 +494,6 @@
   </si>
   <si>
     <t>30358_363</t>
-  </si>
-  <si>
-    <t>30358_401</t>
   </si>
   <si>
     <t>24431_262</t>
@@ -1027,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM156"/>
+  <dimension ref="A1:AM155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M126" sqref="M126"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I144" sqref="I144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1171,13 +1168,13 @@
         <v>1.000000000000167E-4</v>
       </c>
       <c r="G2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J2">
         <v>1668261.222189615</v>
@@ -1266,13 +1263,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H3" t="s">
         <v>192</v>
       </c>
-      <c r="H3" t="s">
-        <v>193</v>
-      </c>
       <c r="I3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J3">
         <v>4250669.025714186</v>
@@ -1361,13 +1358,13 @@
         <v>1.0000000000009999E-5</v>
       </c>
       <c r="G4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J4">
         <v>1765204.192724434</v>
@@ -1456,13 +1453,13 @@
         <v>9.9999999999544897E-6</v>
       </c>
       <c r="G5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H5" t="s">
         <v>192</v>
       </c>
-      <c r="H5" t="s">
-        <v>193</v>
-      </c>
       <c r="I5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J5">
         <v>4282123.0140156886</v>
@@ -1551,13 +1548,13 @@
         <v>9.9999999999544897E-6</v>
       </c>
       <c r="G6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J6">
         <v>2760769.670463996</v>
@@ -1646,13 +1643,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G7" t="s">
+        <v>191</v>
+      </c>
+      <c r="H7" t="s">
         <v>192</v>
       </c>
-      <c r="H7" t="s">
-        <v>193</v>
-      </c>
       <c r="I7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J7">
         <v>1549572.66310395</v>
@@ -1741,13 +1738,13 @@
         <v>1.0000000000009999E-5</v>
       </c>
       <c r="G8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J8">
         <v>1825603.0311702739</v>
@@ -1818,13 +1815,13 @@
         <v>1.0000000000009999E-5</v>
       </c>
       <c r="G9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" t="s">
         <v>192</v>
       </c>
-      <c r="H9" t="s">
-        <v>193</v>
-      </c>
       <c r="I9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J9">
         <v>3120930.232703018</v>
@@ -1913,13 +1910,13 @@
         <v>1.000000000000167E-4</v>
       </c>
       <c r="G10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J10">
         <v>1698319.6733202189</v>
@@ -2008,13 +2005,13 @@
         <v>9.9999999999544897E-6</v>
       </c>
       <c r="G11" t="s">
+        <v>191</v>
+      </c>
+      <c r="H11" t="s">
         <v>192</v>
       </c>
-      <c r="H11" t="s">
-        <v>193</v>
-      </c>
       <c r="I11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J11">
         <v>3190321.6380787082</v>
@@ -2103,13 +2100,13 @@
         <v>1.000000000000167E-4</v>
       </c>
       <c r="G12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J12">
         <v>1671783.5767103841</v>
@@ -2198,13 +2195,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G13" t="s">
+        <v>191</v>
+      </c>
+      <c r="H13" t="s">
         <v>192</v>
       </c>
-      <c r="H13" t="s">
-        <v>193</v>
-      </c>
       <c r="I13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J13">
         <v>4137439.7116720472</v>
@@ -2293,13 +2290,13 @@
         <v>1.000000000000167E-4</v>
       </c>
       <c r="G14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J14">
         <v>1905816.5020364369</v>
@@ -2370,13 +2367,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G15" t="s">
+        <v>191</v>
+      </c>
+      <c r="H15" t="s">
         <v>192</v>
       </c>
-      <c r="H15" t="s">
-        <v>193</v>
-      </c>
       <c r="I15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J15">
         <v>3465540.686422857</v>
@@ -2465,13 +2462,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J16">
         <v>1847058.445973017</v>
@@ -2560,13 +2557,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G17" t="s">
+        <v>191</v>
+      </c>
+      <c r="H17" t="s">
         <v>192</v>
       </c>
-      <c r="H17" t="s">
-        <v>193</v>
-      </c>
       <c r="I17" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J17">
         <v>2200166.120436688</v>
@@ -2655,13 +2652,13 @@
         <v>-9.9999999999988987E-5</v>
       </c>
       <c r="G18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J18">
         <v>-10000000</v>
@@ -2774,13 +2771,13 @@
         <v>6.9999999999986739E-5</v>
       </c>
       <c r="G19" t="s">
+        <v>191</v>
+      </c>
+      <c r="H19" t="s">
         <v>192</v>
       </c>
-      <c r="H19" t="s">
-        <v>193</v>
-      </c>
       <c r="I19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J19">
         <v>-10000000</v>
@@ -2893,13 +2890,13 @@
         <v>1.99999999999978E-4</v>
       </c>
       <c r="G20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J20">
         <v>4004025.2340074959</v>
@@ -3012,13 +3009,13 @@
         <v>2.0000000000003351E-4</v>
       </c>
       <c r="G21" t="s">
+        <v>191</v>
+      </c>
+      <c r="H21" t="s">
         <v>192</v>
       </c>
-      <c r="H21" t="s">
-        <v>193</v>
-      </c>
       <c r="I21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J21">
         <v>7755985.6316315234</v>
@@ -3131,13 +3128,13 @@
         <v>1.5000000000000009E-3</v>
       </c>
       <c r="G22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J22">
         <v>3931351.5319708181</v>
@@ -3250,13 +3247,13 @@
         <v>9.000000000000119E-4</v>
       </c>
       <c r="G23" t="s">
+        <v>191</v>
+      </c>
+      <c r="H23" t="s">
         <v>192</v>
       </c>
-      <c r="H23" t="s">
-        <v>193</v>
-      </c>
       <c r="I23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J23">
         <v>6559111.2237224616</v>
@@ -3369,13 +3366,13 @@
         <v>3.0000000000002253E-4</v>
       </c>
       <c r="G24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J24">
         <v>3781156.3727709712</v>
@@ -3488,13 +3485,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G25" t="s">
+        <v>191</v>
+      </c>
+      <c r="H25" t="s">
         <v>192</v>
       </c>
-      <c r="H25" t="s">
-        <v>193</v>
-      </c>
       <c r="I25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J25">
         <v>4860862.1104128631</v>
@@ -3607,13 +3604,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J26">
         <v>4117624.763061869</v>
@@ -3726,13 +3723,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G27" t="s">
+        <v>191</v>
+      </c>
+      <c r="H27" t="s">
         <v>192</v>
       </c>
-      <c r="H27" t="s">
-        <v>193</v>
-      </c>
       <c r="I27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J27">
         <v>3620410.4107727632</v>
@@ -3845,13 +3842,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J28">
         <v>3807997.356260973</v>
@@ -3964,13 +3961,13 @@
         <v>5.9999999999998943E-4</v>
       </c>
       <c r="G29" t="s">
+        <v>191</v>
+      </c>
+      <c r="H29" t="s">
         <v>192</v>
       </c>
-      <c r="H29" t="s">
-        <v>193</v>
-      </c>
       <c r="I29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J29">
         <v>3927546.9015078731</v>
@@ -4083,13 +4080,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G30" t="s">
+        <v>191</v>
+      </c>
+      <c r="H30" t="s">
         <v>192</v>
       </c>
-      <c r="H30" t="s">
-        <v>193</v>
-      </c>
       <c r="I30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J30">
         <v>4238070.5071030324</v>
@@ -4196,13 +4193,13 @@
         <v>5.0000000000000036E-3</v>
       </c>
       <c r="G31" t="s">
+        <v>191</v>
+      </c>
+      <c r="H31" t="s">
         <v>192</v>
       </c>
-      <c r="H31" t="s">
-        <v>193</v>
-      </c>
       <c r="I31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J31">
         <v>3154913.280887431</v>
@@ -4306,13 +4303,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G32" t="s">
+        <v>191</v>
+      </c>
+      <c r="H32" t="s">
         <v>192</v>
       </c>
-      <c r="H32" t="s">
-        <v>193</v>
-      </c>
       <c r="I32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J32">
         <v>3978311.433844503</v>
@@ -4425,13 +4422,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I33" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J33">
         <v>3115560.7962352489</v>
@@ -4538,13 +4535,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G34" t="s">
+        <v>191</v>
+      </c>
+      <c r="H34" t="s">
         <v>192</v>
       </c>
-      <c r="H34" t="s">
-        <v>193</v>
-      </c>
       <c r="I34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J34">
         <v>3386271.851881268</v>
@@ -4651,13 +4648,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H35" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I35" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J35">
         <v>3416101.118973895</v>
@@ -4770,13 +4767,13 @@
         <v>6.9999999999997842E-4</v>
       </c>
       <c r="G36" t="s">
+        <v>191</v>
+      </c>
+      <c r="H36" t="s">
         <v>192</v>
       </c>
-      <c r="H36" t="s">
-        <v>193</v>
-      </c>
       <c r="I36" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J36">
         <v>5592736.9846213479</v>
@@ -4889,13 +4886,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G37" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I37" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J37">
         <v>267057.33591785328</v>
@@ -4966,13 +4963,13 @@
         <v>3.0000000000000031E-3</v>
       </c>
       <c r="G38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H38" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J38">
         <v>2231106.7458404978</v>
@@ -5043,13 +5040,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J39">
         <v>1574505.922283242</v>
@@ -5120,13 +5117,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J40">
         <v>3077568.9079023688</v>
@@ -5197,13 +5194,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H41" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I41" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J41">
         <v>1761813.084523099</v>
@@ -5274,13 +5271,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I42" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J42">
         <v>2921561.8188902759</v>
@@ -5351,13 +5348,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G43" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H43" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J43">
         <v>2528506.2949038218</v>
@@ -5428,13 +5425,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G44" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I44" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J44">
         <v>2787846.7964247311</v>
@@ -5505,13 +5502,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G45" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I45" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J45">
         <v>207972.10693308589</v>
@@ -5582,13 +5579,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H46" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I46" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J46">
         <v>3340745.85650974</v>
@@ -5659,13 +5656,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G47" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H47" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I47" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J47">
         <v>1654604.7161002781</v>
@@ -5736,13 +5733,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G48" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H48" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J48">
         <v>1685296.976852543</v>
@@ -5813,13 +5810,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G49" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H49" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J49">
         <v>1781739.1987198479</v>
@@ -5890,13 +5887,13 @@
         <v>2.0000000000000022E-3</v>
       </c>
       <c r="G50" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J50">
         <v>579362.1875</v>
@@ -5967,13 +5964,13 @@
         <v>6.0000000000000053E-3</v>
       </c>
       <c r="G51" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H51" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I51" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J51">
         <v>1503462.56778286</v>
@@ -6044,13 +6041,13 @@
         <v>9.9999999999994538E-4</v>
       </c>
       <c r="G52" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H52" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I52" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J52">
         <v>351183.2539847095</v>
@@ -6121,13 +6118,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G53" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I53" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J53">
         <v>2441344.8988700612</v>
@@ -6198,13 +6195,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G54" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H54" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J54">
         <v>2342249.1920747659</v>
@@ -6275,13 +6272,13 @@
         <v>6.9999999999997842E-4</v>
       </c>
       <c r="G55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H55" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I55" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J55">
         <v>2258928.5708549181</v>
@@ -6352,13 +6349,13 @@
         <v>7.0000000000003393E-4</v>
       </c>
       <c r="G56" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H56" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J56">
         <v>1879365.145333187</v>
@@ -6429,13 +6426,13 @@
         <v>4.0000000000001151E-4</v>
       </c>
       <c r="G57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H57" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I57" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J57">
         <v>2230398.1582934549</v>
@@ -6506,13 +6503,13 @@
         <v>4.9999999999994493E-5</v>
       </c>
       <c r="G58" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H58" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J58">
         <v>1924282.5752918939</v>
@@ -6583,13 +6580,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G59" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H59" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I59" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J59">
         <v>1847599.051815737</v>
@@ -6660,13 +6657,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G60" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H60" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I60" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J60">
         <v>1885729.321374509</v>
@@ -6737,13 +6734,13 @@
         <v>2.2999999999999961E-2</v>
       </c>
       <c r="G61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H61" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I61" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J61">
         <v>837384.55940206349</v>
@@ -6814,13 +6811,13 @@
         <v>3.0000000000000031E-3</v>
       </c>
       <c r="G62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H62" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I62" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J62">
         <v>464363.36429925961</v>
@@ -6891,13 +6888,13 @@
         <v>1.99999999999978E-4</v>
       </c>
       <c r="G63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I63" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J63">
         <v>3868866.9241197342</v>
@@ -7010,13 +7007,13 @@
         <v>1.99999999999978E-4</v>
       </c>
       <c r="G64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J64">
         <v>5990410.5100809848</v>
@@ -7129,13 +7126,13 @@
         <v>1.99999999999978E-4</v>
       </c>
       <c r="G65" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H65" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I65" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J65">
         <v>3598295.0932049798</v>
@@ -7248,13 +7245,13 @@
         <v>4.0000000000001151E-4</v>
       </c>
       <c r="G66" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H66" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J66">
         <v>4404047.5705150133</v>
@@ -7367,13 +7364,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G67" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H67" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J67">
         <v>4143492.9420307572</v>
@@ -7486,13 +7483,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G68" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H68" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I68" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J68">
         <v>4592315.252820638</v>
@@ -7605,13 +7602,13 @@
         <v>3.0000000000002253E-4</v>
       </c>
       <c r="G69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H69" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J69">
         <v>3815294.1733383602</v>
@@ -7724,13 +7721,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H70" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I70" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J70">
         <v>3760244.8872812139</v>
@@ -7843,13 +7840,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H71" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I71" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J71">
         <v>3199311.9454879509</v>
@@ -7962,13 +7959,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G72" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I72" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J72">
         <v>3566379.4452871731</v>
@@ -8081,13 +8078,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G73" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H73" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I73" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J73">
         <v>3809146.8795361319</v>
@@ -8200,13 +8197,13 @@
         <v>7.3999999999999622E-3</v>
       </c>
       <c r="G74" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H74" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J74">
         <v>4390461.3102648556</v>
@@ -8319,13 +8316,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G75" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H75" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I75" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J75">
         <v>3737071.4952669689</v>
@@ -8438,13 +8435,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G76" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H76" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I76" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J76">
         <v>6058067.9896562034</v>
@@ -8557,13 +8554,13 @@
         <v>2.7999999999999692E-3</v>
       </c>
       <c r="G77" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H77" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J77">
         <v>2534795.840560324</v>
@@ -8676,13 +8673,13 @@
         <v>5.9999999999998943E-4</v>
       </c>
       <c r="G78" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H78" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J78">
         <v>3073719.2770271678</v>
@@ -8795,13 +8792,13 @@
         <v>8.0000000000002292E-4</v>
       </c>
       <c r="G79" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I79" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J79">
         <v>3653906.9675194342</v>
@@ -8914,13 +8911,13 @@
         <v>4.9999999999994493E-4</v>
       </c>
       <c r="G80" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H80" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I80" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J80">
         <v>5467350.275784188</v>
@@ -9033,13 +9030,13 @@
         <v>2.0000000000003351E-4</v>
       </c>
       <c r="G81" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H81" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I81" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J81">
         <v>3384216.4108965979</v>
@@ -9152,13 +9149,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G82" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H82" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I82" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J82">
         <v>1974859.5</v>
@@ -9271,13 +9268,13 @@
         <v>3.399999999999959E-3</v>
       </c>
       <c r="G83" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J83">
         <v>3564521.3978160941</v>
@@ -9390,13 +9387,13 @@
         <v>4.9999999999994493E-4</v>
       </c>
       <c r="G84" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H84" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I84" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J84">
         <v>4615763.7853525504</v>
@@ -9509,13 +9506,13 @@
         <v>3.9999999999995589E-4</v>
       </c>
       <c r="G85" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H85" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I85" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J85">
         <v>3522082.3843260719</v>
@@ -9628,13 +9625,13 @@
         <v>3.0000000000002253E-4</v>
       </c>
       <c r="G86" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H86" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I86" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J86">
         <v>4254612.6243875055</v>
@@ -9747,13 +9744,13 @@
         <v>1.4000000000000011E-2</v>
       </c>
       <c r="G87" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H87" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I87" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J87">
         <v>3318196.3345566601</v>
@@ -9866,13 +9863,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G88" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H88" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I88" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J88">
         <v>4662553.6321508624</v>
@@ -9985,13 +9982,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G89" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H89" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I89" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J89">
         <v>3887887.3486341462</v>
@@ -10104,13 +10101,13 @@
         <v>1.000000000000445E-4</v>
       </c>
       <c r="G90" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H90" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I90" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J90">
         <v>3545332.7817244958</v>
@@ -10223,13 +10220,13 @@
         <v>3.0000000000002253E-4</v>
       </c>
       <c r="G91" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I91" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J91">
         <v>3390040.9732032898</v>
@@ -10342,13 +10339,13 @@
         <v>1.99999999999978E-4</v>
       </c>
       <c r="G92" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H92" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J92">
         <v>4149469.6894111098</v>
@@ -10461,13 +10458,13 @@
         <v>2.0000000000003351E-4</v>
       </c>
       <c r="G93" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H93" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I93" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J93">
         <v>3633484.8357146611</v>
@@ -10580,13 +10577,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G94" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H94" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J94">
         <v>5816261.6136825662</v>
@@ -10699,13 +10696,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G95" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H95" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J95">
         <v>3593225.946071811</v>
@@ -10818,13 +10815,13 @@
         <v>8.0000000000002292E-4</v>
       </c>
       <c r="G96" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H96" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I96" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J96">
         <v>4433839.3464630377</v>
@@ -10928,13 +10925,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G97" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H97" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I97" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J97">
         <v>3802700.5815977282</v>
@@ -11047,13 +11044,13 @@
         <v>1.0000000000009999E-5</v>
       </c>
       <c r="G98" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H98" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I98" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J98">
         <v>6589369.315586214</v>
@@ -11148,13 +11145,13 @@
         <v>3.0000000000002253E-4</v>
       </c>
       <c r="G99" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H99" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I99" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J99">
         <v>3543285.0441407631</v>
@@ -11267,13 +11264,13 @@
         <v>2.0000000000000022E-3</v>
       </c>
       <c r="G100" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H100" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I100" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J100">
         <v>4002966.8555642422</v>
@@ -11368,13 +11365,13 @@
         <v>2.0000000000003351E-4</v>
       </c>
       <c r="G101" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H101" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J101">
         <v>3495302.0993565689</v>
@@ -11487,13 +11484,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G102" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H102" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I102" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J102">
         <v>4574873.2810473656</v>
@@ -11588,13 +11585,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G103" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H103" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I103" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J103">
         <v>3874651.3547802018</v>
@@ -11707,13 +11704,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G104" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H104" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I104" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J104">
         <v>3586003.8785376418</v>
@@ -11826,13 +11823,13 @@
         <v>2.0000000000003351E-4</v>
       </c>
       <c r="G105" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H105" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I105" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J105">
         <v>3490368.0162398112</v>
@@ -11945,13 +11942,13 @@
         <v>1.000000000000445E-4</v>
       </c>
       <c r="G106" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H106" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I106" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J106">
         <v>3738650.420096023</v>
@@ -12064,13 +12061,13 @@
         <v>4.0000000000001151E-4</v>
       </c>
       <c r="G107" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H107" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I107" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J107">
         <v>3513764.832519657</v>
@@ -12183,13 +12180,13 @@
         <v>1.000000000000445E-4</v>
       </c>
       <c r="G108" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H108" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I108" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J108">
         <v>3622969.5131848929</v>
@@ -12284,13 +12281,13 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G109" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H109" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J109">
         <v>3310849.4937999188</v>
@@ -12403,13 +12400,13 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G110" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H110" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J110">
         <v>4430897.8591801729</v>
@@ -12513,13 +12510,13 @@
         <v>1.99999999999978E-4</v>
       </c>
       <c r="G111" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H111" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I111" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J111">
         <v>3624871.6287669651</v>
@@ -12632,13 +12629,13 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G112" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H112" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I112" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J112">
         <v>6123007.1731590051</v>
@@ -12733,10 +12730,10 @@
         <v>3.400000000000003E-2</v>
       </c>
       <c r="G113" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H113" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I113" t="s">
         <v>198</v>
@@ -12852,10 +12849,10 @@
         <v>2.0000000000000022E-3</v>
       </c>
       <c r="G114" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H114" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I114" t="s">
         <v>198</v>
@@ -12971,13 +12968,13 @@
         <v>2.0000000000000022E-3</v>
       </c>
       <c r="G115" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H115" t="s">
+        <v>196</v>
+      </c>
+      <c r="I115" t="s">
         <v>197</v>
-      </c>
-      <c r="I115" t="s">
-        <v>198</v>
       </c>
       <c r="J115">
         <v>2952242.5077527622</v>
@@ -13090,13 +13087,13 @@
         <v>2.9999999999996701E-4</v>
       </c>
       <c r="G116" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H116" t="s">
+        <v>196</v>
+      </c>
+      <c r="I116" t="s">
         <v>197</v>
-      </c>
-      <c r="I116" t="s">
-        <v>198</v>
       </c>
       <c r="J116">
         <v>3257597.1088831732</v>
@@ -13209,10 +13206,10 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G117" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H117" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I117" t="s">
         <v>198</v>
@@ -13328,10 +13325,10 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G118" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H118" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I118" t="s">
         <v>198</v>
@@ -13447,10 +13444,10 @@
         <v>5.0000000000000044E-4</v>
       </c>
       <c r="G119" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H119" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I119" t="s">
         <v>198</v>
@@ -13566,10 +13563,10 @@
         <v>1.5000000000000009E-3</v>
       </c>
       <c r="G120" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H120" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I120" t="s">
         <v>198</v>
@@ -13685,10 +13682,10 @@
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G121" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H121" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I121" t="s">
         <v>198</v>
@@ -13789,58 +13786,58 @@
         <v>125</v>
       </c>
       <c r="B122">
-        <v>30358</v>
+        <v>24431</v>
       </c>
       <c r="C122" t="s">
         <v>158</v>
       </c>
       <c r="D122">
-        <v>0.40100000000000002</v>
+        <v>0.26150000000000001</v>
       </c>
       <c r="E122">
-        <v>-1.0000000000000011E-3</v>
+        <v>-5.0000000000000044E-4</v>
       </c>
       <c r="F122">
-        <v>3.0000000000000031E-3</v>
+        <v>5.0000000000000044E-4</v>
       </c>
       <c r="G122" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H122" t="s">
+        <v>196</v>
+      </c>
+      <c r="I122" t="s">
         <v>197</v>
       </c>
-      <c r="I122" t="s">
-        <v>198</v>
-      </c>
       <c r="J122">
-        <v>4920405</v>
+        <v>1977361.64236664</v>
       </c>
       <c r="K122">
-        <v>86371.296875</v>
+        <v>83674.692706667556</v>
       </c>
       <c r="L122">
-        <v>-0.41026455163955688</v>
+        <v>-0.44279336106153327</v>
       </c>
       <c r="M122">
-        <v>0</v>
+        <v>2.0709057530454711E-4</v>
       </c>
       <c r="N122">
-        <v>-0.2318886596223583</v>
+        <v>-0.25027450842608412</v>
       </c>
       <c r="O122">
-        <v>0</v>
+        <v>1.170511947373165E-4</v>
       </c>
       <c r="P122">
-        <v>-0.14363615487771689</v>
+        <v>760.77464802720419</v>
       </c>
       <c r="Q122">
-        <v>40.16068883197719</v>
+        <v>2.2112299523929551</v>
       </c>
       <c r="R122">
-        <v>1.5448131561279299</v>
+        <v>1.882772978963871</v>
       </c>
       <c r="S122">
-        <v>0</v>
+        <v>7.991321555445019E-4</v>
       </c>
       <c r="T122">
         <v>3.1739846250591158E+19</v>
@@ -13914,52 +13911,52 @@
         <v>159</v>
       </c>
       <c r="D123">
-        <v>0.26150000000000001</v>
+        <v>0.38229999999999997</v>
       </c>
       <c r="E123">
-        <v>-5.0000000000000044E-4</v>
+        <v>-2.9999999999996701E-4</v>
       </c>
       <c r="F123">
-        <v>5.0000000000000044E-4</v>
+        <v>5.4000000000000159E-3</v>
       </c>
       <c r="G123" t="s">
         <v>191</v>
       </c>
       <c r="H123" t="s">
+        <v>196</v>
+      </c>
+      <c r="I123" t="s">
         <v>197</v>
       </c>
-      <c r="I123" t="s">
-        <v>198</v>
-      </c>
       <c r="J123">
-        <v>1977361.64236664</v>
+        <v>4094908.9750067061</v>
       </c>
       <c r="K123">
-        <v>83674.692706667556</v>
+        <v>1124802.0652167739</v>
       </c>
       <c r="L123">
-        <v>-0.44279336106153327</v>
+        <v>-0.44624609188893438</v>
       </c>
       <c r="M123">
-        <v>2.0709057530454711E-4</v>
+        <v>7.2839529376944601E-3</v>
       </c>
       <c r="N123">
-        <v>-0.25027450842608412</v>
+        <v>-0.25222605193722392</v>
       </c>
       <c r="O123">
-        <v>1.170511947373165E-4</v>
+        <v>4.1170168778272842E-3</v>
       </c>
       <c r="P123">
-        <v>760.77464802720419</v>
+        <v>759.4342834709513</v>
       </c>
       <c r="Q123">
-        <v>2.2112299523929551</v>
+        <v>14.7081890255663</v>
       </c>
       <c r="R123">
-        <v>1.882772978963871</v>
+        <v>1.8967865702626889</v>
       </c>
       <c r="S123">
-        <v>7.991321555445019E-4</v>
+        <v>2.435365976978621E-2</v>
       </c>
       <c r="T123">
         <v>3.3015661142752821E+19</v>
@@ -14027,58 +14024,58 @@
         <v>127</v>
       </c>
       <c r="B124">
-        <v>24431</v>
+        <v>24514</v>
       </c>
       <c r="C124" t="s">
         <v>160</v>
       </c>
       <c r="D124">
-        <v>0.38229999999999997</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="E124">
-        <v>-2.9999999999996701E-4</v>
+        <v>-1.0000000000000011E-3</v>
       </c>
       <c r="F124">
-        <v>5.4000000000000159E-3</v>
+        <v>1.0000000000000011E-3</v>
       </c>
       <c r="G124" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H124" t="s">
+        <v>196</v>
+      </c>
+      <c r="I124" t="s">
         <v>197</v>
       </c>
-      <c r="I124" t="s">
-        <v>198</v>
-      </c>
       <c r="J124">
-        <v>4094908.9750067061</v>
+        <v>2440624.4604796022</v>
       </c>
       <c r="K124">
-        <v>1124802.0652167739</v>
+        <v>140355.10981433131</v>
       </c>
       <c r="L124">
-        <v>-0.44624609188893438</v>
+        <v>-0.44483105925436411</v>
       </c>
       <c r="M124">
-        <v>7.2839529376944601E-3</v>
+        <v>2.5638213538531351E-4</v>
       </c>
       <c r="N124">
-        <v>-0.25222605193722392</v>
+        <v>-0.25142625088290149</v>
       </c>
       <c r="O124">
-        <v>4.1170168778272842E-3</v>
+        <v>1.449116417395202E-4</v>
       </c>
       <c r="P124">
-        <v>759.4342834709513</v>
+        <v>756.25872020029431</v>
       </c>
       <c r="Q124">
-        <v>14.7081890255663</v>
+        <v>3.428991626270204</v>
       </c>
       <c r="R124">
-        <v>1.8967865702626889</v>
+        <v>1.8532501197303419</v>
       </c>
       <c r="S124">
-        <v>2.435365976978621E-2</v>
+        <v>2.8447962425426349E-4</v>
       </c>
       <c r="T124">
         <v>4.6450710840443544E+19</v>
@@ -14152,52 +14149,52 @@
         <v>161</v>
       </c>
       <c r="D125">
-        <v>0.33600000000000002</v>
+        <v>0.3574</v>
       </c>
       <c r="E125">
-        <v>-1.0000000000000011E-3</v>
+        <v>-4.0000000000001151E-4</v>
       </c>
       <c r="F125">
-        <v>1.0000000000000011E-3</v>
+        <v>9.9999999999988987E-5</v>
       </c>
       <c r="G125" t="s">
         <v>191</v>
       </c>
       <c r="H125" t="s">
+        <v>196</v>
+      </c>
+      <c r="I125" t="s">
         <v>197</v>
       </c>
-      <c r="I125" t="s">
-        <v>198</v>
-      </c>
       <c r="J125">
-        <v>2440624.4604796022</v>
+        <v>4490143.6846102485</v>
       </c>
       <c r="K125">
-        <v>140355.10981433131</v>
+        <v>132267.11168017311</v>
       </c>
       <c r="L125">
-        <v>-0.44483105925436411</v>
+        <v>-0.44470764190225359</v>
       </c>
       <c r="M125">
-        <v>2.5638213538531351E-4</v>
+        <v>2.404870896215994E-4</v>
       </c>
       <c r="N125">
-        <v>-0.25142625088290149</v>
+        <v>-0.25135649324909992</v>
       </c>
       <c r="O125">
-        <v>1.449116417395202E-4</v>
+        <v>1.3592748543828079E-4</v>
       </c>
       <c r="P125">
-        <v>756.25872020029431</v>
+        <v>745.7000066534282</v>
       </c>
       <c r="Q125">
-        <v>3.428991626270204</v>
+        <v>12.659209360755311</v>
       </c>
       <c r="R125">
-        <v>1.8532501197303419</v>
+        <v>1.8479724380057829</v>
       </c>
       <c r="S125">
-        <v>2.8447962425426349E-4</v>
+        <v>2.8514889254465099E-3</v>
       </c>
       <c r="T125">
         <v>3.5914872992295719E+19</v>
@@ -14265,58 +14262,58 @@
         <v>129</v>
       </c>
       <c r="B126">
-        <v>24514</v>
+        <v>24517</v>
       </c>
       <c r="C126" t="s">
         <v>162</v>
       </c>
       <c r="D126">
-        <v>0.3574</v>
+        <v>0.27939999999999998</v>
       </c>
       <c r="E126">
-        <v>-4.0000000000001151E-4</v>
+        <v>6.0000000000004494E-4</v>
       </c>
       <c r="F126">
-        <v>9.9999999999988987E-5</v>
+        <v>5.5999999999999939E-3</v>
       </c>
       <c r="G126" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H126" t="s">
+        <v>196</v>
+      </c>
+      <c r="I126" t="s">
         <v>197</v>
       </c>
-      <c r="I126" t="s">
-        <v>198</v>
-      </c>
       <c r="J126">
-        <v>4490143.6846102485</v>
+        <v>2137204.6121289181</v>
       </c>
       <c r="K126">
-        <v>132267.11168017311</v>
+        <v>224334.35812969241</v>
       </c>
       <c r="L126">
-        <v>-0.44470764190225359</v>
+        <v>-0.44499866005308231</v>
       </c>
       <c r="M126">
-        <v>2.404870896215994E-4</v>
+        <v>1.283348113226668E-3</v>
       </c>
       <c r="N126">
-        <v>-0.25135649324909992</v>
+        <v>-0.25152098176913351</v>
       </c>
       <c r="O126">
-        <v>1.3592748543828079E-4</v>
+        <v>7.2537067269334843E-4</v>
       </c>
       <c r="P126">
-        <v>745.7000066534282</v>
+        <v>766.07931312527933</v>
       </c>
       <c r="Q126">
-        <v>12.659209360755311</v>
+        <v>8.3084974709355492</v>
       </c>
       <c r="R126">
-        <v>1.8479724380057829</v>
+        <v>1.8507513125866011</v>
       </c>
       <c r="S126">
-        <v>2.8514889254465099E-3</v>
+        <v>1.2924912848947701E-2</v>
       </c>
       <c r="T126">
         <v>3.7566605087087247E+19</v>
@@ -14390,52 +14387,52 @@
         <v>163</v>
       </c>
       <c r="D127">
-        <v>0.27939999999999998</v>
+        <v>0.30859999999999999</v>
       </c>
       <c r="E127">
-        <v>6.0000000000004494E-4</v>
+        <v>-8.5999999999999965E-3</v>
       </c>
       <c r="F127">
-        <v>5.5999999999999939E-3</v>
+        <v>-7.5999999999999956E-3</v>
       </c>
       <c r="G127" t="s">
         <v>191</v>
       </c>
       <c r="H127" t="s">
+        <v>196</v>
+      </c>
+      <c r="I127" t="s">
         <v>197</v>
       </c>
-      <c r="I127" t="s">
-        <v>198</v>
-      </c>
       <c r="J127">
-        <v>2137204.6121289181</v>
+        <v>4061115.8141139369</v>
       </c>
       <c r="K127">
-        <v>224334.35812969241</v>
+        <v>297244.91813643719</v>
       </c>
       <c r="L127">
-        <v>-0.44499866005308231</v>
+        <v>-0.44407075308570448</v>
       </c>
       <c r="M127">
-        <v>1.283348113226668E-3</v>
+        <v>2.441090044285998E-3</v>
       </c>
       <c r="N127">
-        <v>-0.25152098176913351</v>
+        <v>-0.25099651261365907</v>
       </c>
       <c r="O127">
-        <v>7.2537067269334843E-4</v>
+        <v>1.379746546770366E-3</v>
       </c>
       <c r="P127">
-        <v>766.07931312527933</v>
+        <v>767.48165262531177</v>
       </c>
       <c r="Q127">
-        <v>8.3084974709355492</v>
+        <v>3.3454225333301788</v>
       </c>
       <c r="R127">
-        <v>1.8507513125866011</v>
+        <v>1.8626279278583571</v>
       </c>
       <c r="S127">
-        <v>1.2924912848947701E-2</v>
+        <v>7.4212179552133328E-3</v>
       </c>
       <c r="T127">
         <v>2.8856338658932199E+19</v>
@@ -14503,58 +14500,58 @@
         <v>131</v>
       </c>
       <c r="B128">
-        <v>24517</v>
+        <v>24518</v>
       </c>
       <c r="C128" t="s">
         <v>164</v>
       </c>
       <c r="D128">
-        <v>0.30859999999999999</v>
+        <v>0.29070000000000001</v>
       </c>
       <c r="E128">
-        <v>-8.5999999999999965E-3</v>
+        <v>-7.0000000000003393E-4</v>
       </c>
       <c r="F128">
-        <v>-7.5999999999999956E-3</v>
+        <v>1.2999999999999681E-3</v>
       </c>
       <c r="G128" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H128" t="s">
+        <v>196</v>
+      </c>
+      <c r="I128" t="s">
         <v>197</v>
       </c>
-      <c r="I128" t="s">
-        <v>198</v>
-      </c>
       <c r="J128">
-        <v>4061115.8141139369</v>
+        <v>2203839.596586606</v>
       </c>
       <c r="K128">
-        <v>297244.91813643719</v>
+        <v>97346.55472681376</v>
       </c>
       <c r="L128">
-        <v>-0.44407075308570448</v>
+        <v>-0.4443614717241538</v>
       </c>
       <c r="M128">
-        <v>2.441090044285998E-3</v>
+        <v>3.5457644899034019E-4</v>
       </c>
       <c r="N128">
-        <v>-0.25099651261365907</v>
+        <v>-0.25116083184408688</v>
       </c>
       <c r="O128">
-        <v>1.379746546770366E-3</v>
+        <v>2.0041277551630099E-4</v>
       </c>
       <c r="P128">
-        <v>767.48165262531177</v>
+        <v>761.86142461042266</v>
       </c>
       <c r="Q128">
-        <v>3.3454225333301788</v>
+        <v>3.7971831916177048</v>
       </c>
       <c r="R128">
-        <v>1.8626279278583571</v>
+        <v>1.842038413614443</v>
       </c>
       <c r="S128">
-        <v>7.4212179552133328E-3</v>
+        <v>6.6865984788879729E-3</v>
       </c>
       <c r="T128">
         <v>2.8135567525304652E+19</v>
@@ -14628,52 +14625,52 @@
         <v>165</v>
       </c>
       <c r="D129">
-        <v>0.29070000000000001</v>
+        <v>0.35349999999999998</v>
       </c>
       <c r="E129">
-        <v>-7.0000000000003393E-4</v>
+        <v>-5.0000000000000044E-4</v>
       </c>
       <c r="F129">
-        <v>1.2999999999999681E-3</v>
+        <v>1.000000000000445E-4</v>
       </c>
       <c r="G129" t="s">
         <v>191</v>
       </c>
       <c r="H129" t="s">
+        <v>196</v>
+      </c>
+      <c r="I129" t="s">
         <v>197</v>
       </c>
-      <c r="I129" t="s">
-        <v>198</v>
-      </c>
       <c r="J129">
-        <v>2203839.596586606</v>
+        <v>3425603.599309809</v>
       </c>
       <c r="K129">
-        <v>97346.55472681376</v>
+        <v>202125.27616272969</v>
       </c>
       <c r="L129">
-        <v>-0.4443614717241538</v>
+        <v>-0.43846139352624819</v>
       </c>
       <c r="M129">
-        <v>3.5457644899034019E-4</v>
+        <v>4.1096488090985872E-4</v>
       </c>
       <c r="N129">
-        <v>-0.25116083184408688</v>
+        <v>-0.24782600503657509</v>
       </c>
       <c r="O129">
-        <v>2.0041277551630099E-4</v>
+        <v>2.3228449790557709E-4</v>
       </c>
       <c r="P129">
-        <v>761.86142461042266</v>
+        <v>761.93767118069559</v>
       </c>
       <c r="Q129">
-        <v>3.7971831916177048</v>
+        <v>23.12725657737144</v>
       </c>
       <c r="R129">
-        <v>1.842038413614443</v>
+        <v>1.862908426455645</v>
       </c>
       <c r="S129">
-        <v>6.6865984788879729E-3</v>
+        <v>1.3120520706675349E-3</v>
       </c>
       <c r="T129">
         <v>2.729337468614203E+19</v>
@@ -14741,58 +14738,58 @@
         <v>133</v>
       </c>
       <c r="B130">
-        <v>24518</v>
+        <v>24522</v>
       </c>
       <c r="C130" t="s">
         <v>166</v>
       </c>
       <c r="D130">
-        <v>0.35349999999999998</v>
+        <v>0.2535</v>
       </c>
       <c r="E130">
         <v>-5.0000000000000044E-4</v>
       </c>
       <c r="F130">
-        <v>1.000000000000445E-4</v>
+        <v>5.0000000000000044E-4</v>
       </c>
       <c r="G130" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H130" t="s">
+        <v>196</v>
+      </c>
+      <c r="I130" t="s">
         <v>197</v>
       </c>
-      <c r="I130" t="s">
-        <v>198</v>
-      </c>
       <c r="J130">
-        <v>3425603.599309809</v>
+        <v>2140970.326732161</v>
       </c>
       <c r="K130">
-        <v>202125.27616272969</v>
+        <v>118883.07280894381</v>
       </c>
       <c r="L130">
-        <v>-0.43846139352624819</v>
+        <v>-0.44887132626513998</v>
       </c>
       <c r="M130">
-        <v>4.1096488090985872E-4</v>
+        <v>8.3851298190401602E-4</v>
       </c>
       <c r="N130">
-        <v>-0.24782600503657509</v>
+        <v>-0.25370988006290518</v>
       </c>
       <c r="O130">
-        <v>2.3228449790557709E-4</v>
+        <v>4.739421202066274E-4</v>
       </c>
       <c r="P130">
-        <v>761.93767118069559</v>
+        <v>903.4674250462092</v>
       </c>
       <c r="Q130">
-        <v>23.12725657737144</v>
+        <v>3.184121868963302</v>
       </c>
       <c r="R130">
-        <v>1.862908426455645</v>
+        <v>1.9790949850106729</v>
       </c>
       <c r="S130">
-        <v>1.3120520706675349E-3</v>
+        <v>1.157215745177975E-2</v>
       </c>
       <c r="T130">
         <v>3.2506834564725449E+19</v>
@@ -14866,52 +14863,52 @@
         <v>167</v>
       </c>
       <c r="D131">
-        <v>0.2535</v>
+        <v>0.35549999999999998</v>
       </c>
       <c r="E131">
         <v>-5.0000000000000044E-4</v>
       </c>
       <c r="F131">
-        <v>5.0000000000000044E-4</v>
+        <v>3.0000000000002253E-4</v>
       </c>
       <c r="G131" t="s">
         <v>191</v>
       </c>
       <c r="H131" t="s">
+        <v>196</v>
+      </c>
+      <c r="I131" t="s">
         <v>197</v>
       </c>
-      <c r="I131" t="s">
-        <v>198</v>
-      </c>
       <c r="J131">
-        <v>2140970.326732161</v>
+        <v>4286318.6141580446</v>
       </c>
       <c r="K131">
-        <v>118883.07280894381</v>
+        <v>196360.4221986208</v>
       </c>
       <c r="L131">
-        <v>-0.44887132626513998</v>
+        <v>-0.45559527509083692</v>
       </c>
       <c r="M131">
-        <v>8.3851298190401602E-4</v>
+        <v>1.65014424337806E-4</v>
       </c>
       <c r="N131">
-        <v>-0.25370988006290518</v>
+        <v>-0.25751037287742962</v>
       </c>
       <c r="O131">
-        <v>4.739421202066274E-4</v>
+        <v>9.3269022451825112E-5</v>
       </c>
       <c r="P131">
-        <v>903.4674250462092</v>
+        <v>884.2487419226992</v>
       </c>
       <c r="Q131">
-        <v>3.184121868963302</v>
+        <v>3.736321825054119</v>
       </c>
       <c r="R131">
-        <v>1.9790949850106729</v>
+        <v>1.887135499308203</v>
       </c>
       <c r="S131">
-        <v>1.157215745177975E-2</v>
+        <v>1.0609198197554241E-2</v>
       </c>
       <c r="T131">
         <v>2.9467848341089489E+19</v>
@@ -14979,58 +14976,58 @@
         <v>135</v>
       </c>
       <c r="B132">
-        <v>24522</v>
+        <v>24524</v>
       </c>
       <c r="C132" t="s">
         <v>168</v>
       </c>
       <c r="D132">
-        <v>0.35549999999999998</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="E132">
-        <v>-5.0000000000000044E-4</v>
+        <v>-4.0000000000000044E-3</v>
       </c>
       <c r="F132">
-        <v>3.0000000000002253E-4</v>
+        <v>1.0000000000000011E-3</v>
       </c>
       <c r="G132" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H132" t="s">
+        <v>196</v>
+      </c>
+      <c r="I132" t="s">
         <v>197</v>
       </c>
-      <c r="I132" t="s">
-        <v>198</v>
-      </c>
       <c r="J132">
-        <v>4286318.6141580446</v>
+        <v>1622312.709533545</v>
       </c>
       <c r="K132">
-        <v>196360.4221986208</v>
+        <v>70430.41415599882</v>
       </c>
       <c r="L132">
-        <v>-0.45559527509083692</v>
+        <v>-0.40327608390121172</v>
       </c>
       <c r="M132">
-        <v>1.65014424337806E-4</v>
+        <v>8.6690796126137615E-4</v>
       </c>
       <c r="N132">
-        <v>-0.25751037287742962</v>
+        <v>-0.2279386561180762</v>
       </c>
       <c r="O132">
-        <v>9.3269022451825112E-5</v>
+        <v>4.899914563651353E-4</v>
       </c>
       <c r="P132">
-        <v>884.2487419226992</v>
+        <v>796.84579437248578</v>
       </c>
       <c r="Q132">
-        <v>3.736321825054119</v>
+        <v>6.4084561251693231</v>
       </c>
       <c r="R132">
-        <v>1.887135499308203</v>
+        <v>2.0079763363625469</v>
       </c>
       <c r="S132">
-        <v>1.0609198197554241E-2</v>
+        <v>1.3348593644470609E-2</v>
       </c>
       <c r="T132">
         <v>3.9186850095609078E+19</v>
@@ -15104,52 +15101,52 @@
         <v>169</v>
       </c>
       <c r="D133">
-        <v>0.20100000000000001</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="E133">
-        <v>-4.0000000000000044E-3</v>
+        <v>-1.0000000000000011E-3</v>
       </c>
       <c r="F133">
-        <v>1.0000000000000011E-3</v>
+        <v>8.0000000000002292E-4</v>
       </c>
       <c r="G133" t="s">
         <v>191</v>
       </c>
       <c r="H133" t="s">
+        <v>196</v>
+      </c>
+      <c r="I133" t="s">
         <v>197</v>
       </c>
-      <c r="I133" t="s">
-        <v>198</v>
-      </c>
       <c r="J133">
-        <v>1622312.709533545</v>
+        <v>2372374.265079394</v>
       </c>
       <c r="K133">
-        <v>70430.41415599882</v>
+        <v>69336.261832051096</v>
       </c>
       <c r="L133">
-        <v>-0.40327608390121172</v>
+        <v>-0.4014418134507034</v>
       </c>
       <c r="M133">
-        <v>8.6690796126137615E-4</v>
+        <v>4.4477505185608329E-4</v>
       </c>
       <c r="N133">
-        <v>-0.2279386561180762</v>
+        <v>-0.22690189455909329</v>
       </c>
       <c r="O133">
-        <v>4.899914563651353E-4</v>
+        <v>2.513945945273599E-4</v>
       </c>
       <c r="P133">
-        <v>796.84579437248578</v>
+        <v>789.61966587944164</v>
       </c>
       <c r="Q133">
-        <v>6.4084561251693231</v>
+        <v>5.6365602376829429</v>
       </c>
       <c r="R133">
-        <v>2.0079763363625469</v>
+        <v>1.939839431315854</v>
       </c>
       <c r="S133">
-        <v>1.3348593644470609E-2</v>
+        <v>4.1359222895300807E-3</v>
       </c>
       <c r="T133">
         <v>2.4027434221258142E+19</v>
@@ -15220,55 +15217,55 @@
         <v>24524</v>
       </c>
       <c r="C134" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D134">
-        <v>0.35499999999999998</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="E134">
-        <v>-1.0000000000000011E-3</v>
+        <v>-4.0000000000000044E-3</v>
       </c>
       <c r="F134">
-        <v>8.0000000000002292E-4</v>
+        <v>1.0000000000000011E-3</v>
       </c>
       <c r="G134" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H134" t="s">
+        <v>196</v>
+      </c>
+      <c r="I134" t="s">
         <v>197</v>
       </c>
-      <c r="I134" t="s">
-        <v>198</v>
-      </c>
       <c r="J134">
-        <v>2372374.265079394</v>
+        <v>1622312.709533545</v>
       </c>
       <c r="K134">
-        <v>69336.261832051096</v>
+        <v>70430.41415599882</v>
       </c>
       <c r="L134">
-        <v>-0.4014418134507034</v>
+        <v>-0.40327608390121172</v>
       </c>
       <c r="M134">
-        <v>4.4477505185608329E-4</v>
+        <v>8.6690796126137615E-4</v>
       </c>
       <c r="N134">
-        <v>-0.22690189455909329</v>
+        <v>-0.2279386561180762</v>
       </c>
       <c r="O134">
-        <v>2.513945945273599E-4</v>
+        <v>4.899914563651353E-4</v>
       </c>
       <c r="P134">
-        <v>789.61966587944164</v>
+        <v>796.84579437248578</v>
       </c>
       <c r="Q134">
-        <v>5.6365602376829429</v>
+        <v>6.4084561251693231</v>
       </c>
       <c r="R134">
-        <v>1.939839431315854</v>
+        <v>2.0079763363625469</v>
       </c>
       <c r="S134">
-        <v>4.1359222895300807E-3</v>
+        <v>1.3348593644470609E-2</v>
       </c>
       <c r="T134">
         <v>4.1399095990659932E+19</v>
@@ -15342,52 +15339,52 @@
         <v>169</v>
       </c>
       <c r="D135">
-        <v>0.20100000000000001</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="E135">
-        <v>-4.0000000000000044E-3</v>
+        <v>-1.0000000000000011E-3</v>
       </c>
       <c r="F135">
-        <v>1.0000000000000011E-3</v>
+        <v>8.0000000000002292E-4</v>
       </c>
       <c r="G135" t="s">
         <v>191</v>
       </c>
       <c r="H135" t="s">
+        <v>196</v>
+      </c>
+      <c r="I135" t="s">
         <v>197</v>
       </c>
-      <c r="I135" t="s">
-        <v>198</v>
-      </c>
       <c r="J135">
-        <v>1622312.709533545</v>
+        <v>2372374.265079394</v>
       </c>
       <c r="K135">
-        <v>70430.41415599882</v>
+        <v>69336.261832051096</v>
       </c>
       <c r="L135">
-        <v>-0.40327608390121172</v>
+        <v>-0.4014418134507034</v>
       </c>
       <c r="M135">
-        <v>8.6690796126137615E-4</v>
+        <v>4.4477505185608329E-4</v>
       </c>
       <c r="N135">
-        <v>-0.2279386561180762</v>
+        <v>-0.22690189455909329</v>
       </c>
       <c r="O135">
-        <v>4.899914563651353E-4</v>
+        <v>2.513945945273599E-4</v>
       </c>
       <c r="P135">
-        <v>796.84579437248578</v>
+        <v>789.61966587944164</v>
       </c>
       <c r="Q135">
-        <v>6.4084561251693231</v>
+        <v>5.6365602376829429</v>
       </c>
       <c r="R135">
-        <v>2.0079763363625469</v>
+        <v>1.939839431315854</v>
       </c>
       <c r="S135">
-        <v>1.3348593644470609E-2</v>
+        <v>4.1359222895300807E-3</v>
       </c>
       <c r="T135">
         <v>2.4027434221258142E+19</v>
@@ -15455,58 +15452,58 @@
         <v>139</v>
       </c>
       <c r="B136">
-        <v>24524</v>
+        <v>29486</v>
       </c>
       <c r="C136" t="s">
         <v>170</v>
       </c>
       <c r="D136">
-        <v>0.35499999999999998</v>
+        <v>0.2681</v>
       </c>
       <c r="E136">
-        <v>-1.0000000000000011E-3</v>
+        <v>-9.9999999999988987E-5</v>
       </c>
       <c r="F136">
-        <v>8.0000000000002292E-4</v>
+        <v>9.9999999999988987E-5</v>
       </c>
       <c r="G136" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H136" t="s">
+        <v>196</v>
+      </c>
+      <c r="I136" t="s">
         <v>197</v>
       </c>
-      <c r="I136" t="s">
-        <v>198</v>
-      </c>
       <c r="J136">
-        <v>2372374.265079394</v>
+        <v>3413002.8845568029</v>
       </c>
       <c r="K136">
-        <v>69336.261832051096</v>
+        <v>54352.078709341331</v>
       </c>
       <c r="L136">
-        <v>-0.4014418134507034</v>
+        <v>-0.42924002519319387</v>
       </c>
       <c r="M136">
-        <v>4.4477505185608329E-4</v>
+        <v>5.8782156736603142E-6</v>
       </c>
       <c r="N136">
-        <v>-0.22690189455909329</v>
+        <v>-0.24261392728310971</v>
       </c>
       <c r="O136">
-        <v>2.513945945273599E-4</v>
+        <v>3.322469728589406E-6</v>
       </c>
       <c r="P136">
-        <v>789.61966587944164</v>
+        <v>902.50803806603381</v>
       </c>
       <c r="Q136">
-        <v>5.6365602376829429</v>
+        <v>1.123449521146654</v>
       </c>
       <c r="R136">
-        <v>1.939839431315854</v>
+        <v>1.842437394896064</v>
       </c>
       <c r="S136">
-        <v>4.1359222895300807E-3</v>
+        <v>3.1634313234625289E-3</v>
       </c>
       <c r="T136">
         <v>4.1399095990659932E+19</v>
@@ -15580,10 +15577,10 @@
         <v>171</v>
       </c>
       <c r="D137">
-        <v>0.2681</v>
+        <v>0.33779999999999999</v>
       </c>
       <c r="E137">
-        <v>-9.9999999999988987E-5</v>
+        <v>-2.9999999999996701E-4</v>
       </c>
       <c r="F137">
         <v>9.9999999999988987E-5</v>
@@ -15592,40 +15589,40 @@
         <v>191</v>
       </c>
       <c r="H137" t="s">
+        <v>196</v>
+      </c>
+      <c r="I137" t="s">
         <v>197</v>
       </c>
-      <c r="I137" t="s">
-        <v>198</v>
-      </c>
       <c r="J137">
-        <v>3413002.8845568029</v>
+        <v>1985244.7449256789</v>
       </c>
       <c r="K137">
-        <v>54352.078709341331</v>
+        <v>194679.87768830659</v>
       </c>
       <c r="L137">
-        <v>-0.42924002519319387</v>
+        <v>-0.41670290283110628</v>
       </c>
       <c r="M137">
-        <v>5.8782156736603142E-6</v>
+        <v>3.569728144575679E-4</v>
       </c>
       <c r="N137">
-        <v>-0.24261392728310971</v>
+        <v>-0.23552772768714711</v>
       </c>
       <c r="O137">
-        <v>3.322469728589406E-6</v>
+        <v>2.0176724295425941E-4</v>
       </c>
       <c r="P137">
-        <v>902.50803806603381</v>
+        <v>897.41957959950412</v>
       </c>
       <c r="Q137">
-        <v>1.123449521146654</v>
+        <v>10.406912314696569</v>
       </c>
       <c r="R137">
-        <v>1.842437394896064</v>
+        <v>1.8623605355216231</v>
       </c>
       <c r="S137">
-        <v>3.1634313234625289E-3</v>
+        <v>5.5951219802943264E-3</v>
       </c>
       <c r="T137">
         <v>2.969439801930931E+19</v>
@@ -15693,58 +15690,58 @@
         <v>141</v>
       </c>
       <c r="B138">
-        <v>29486</v>
+        <v>29487</v>
       </c>
       <c r="C138" t="s">
         <v>172</v>
       </c>
       <c r="D138">
-        <v>0.33779999999999999</v>
+        <v>0.27250000000000002</v>
       </c>
       <c r="E138">
-        <v>-2.9999999999996701E-4</v>
+        <v>-1.000000000000445E-4</v>
       </c>
       <c r="F138">
         <v>9.9999999999988987E-5</v>
       </c>
       <c r="G138" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H138" t="s">
+        <v>196</v>
+      </c>
+      <c r="I138" t="s">
         <v>197</v>
       </c>
-      <c r="I138" t="s">
-        <v>198</v>
-      </c>
       <c r="J138">
-        <v>1985244.7449256789</v>
+        <v>998789.2308624204</v>
       </c>
       <c r="K138">
-        <v>194679.87768830659</v>
+        <v>419.37095842561371</v>
       </c>
       <c r="L138">
-        <v>-0.41670290283110628</v>
+        <v>-0.44931778217039431</v>
       </c>
       <c r="M138">
-        <v>3.569728144575679E-4</v>
+        <v>2.8884266240702949E-5</v>
       </c>
       <c r="N138">
-        <v>-0.23552772768714711</v>
+        <v>-0.25396222470500551</v>
       </c>
       <c r="O138">
-        <v>2.0176724295425941E-4</v>
+        <v>1.6325889614310359E-5</v>
       </c>
       <c r="P138">
-        <v>897.41957959950412</v>
+        <v>902.87971044165306</v>
       </c>
       <c r="Q138">
-        <v>10.406912314696569</v>
+        <v>3.1989730845907623E-2</v>
       </c>
       <c r="R138">
-        <v>1.8623605355216231</v>
+        <v>1.9348118221216299</v>
       </c>
       <c r="S138">
-        <v>5.5951219802943264E-3</v>
+        <v>2.562033223463267E-4</v>
       </c>
       <c r="T138">
         <v>4.3166720942879801E+19</v>
@@ -15818,52 +15815,52 @@
         <v>173</v>
       </c>
       <c r="D139">
-        <v>0.27250000000000002</v>
+        <v>0.378</v>
       </c>
       <c r="E139">
-        <v>-1.000000000000445E-4</v>
+        <v>-6.0000000000000053E-3</v>
       </c>
       <c r="F139">
-        <v>9.9999999999988987E-5</v>
+        <v>7.0000000000000062E-3</v>
       </c>
       <c r="G139" t="s">
         <v>191</v>
       </c>
       <c r="H139" t="s">
+        <v>196</v>
+      </c>
+      <c r="I139" t="s">
         <v>197</v>
       </c>
-      <c r="I139" t="s">
-        <v>198</v>
-      </c>
       <c r="J139">
-        <v>998789.2308624204</v>
+        <v>879670.00269436976</v>
       </c>
       <c r="K139">
-        <v>419.37095842561371</v>
+        <v>81495.275520363808</v>
       </c>
       <c r="L139">
-        <v>-0.44931778217039431</v>
+        <v>-0.4387348172057895</v>
       </c>
       <c r="M139">
-        <v>2.8884266240702949E-5</v>
+        <v>2.1987985720624552E-3</v>
       </c>
       <c r="N139">
-        <v>-0.25396222470500551</v>
+        <v>-0.24798054885544629</v>
       </c>
       <c r="O139">
-        <v>1.6325889614310359E-5</v>
+        <v>1.2427991929048481E-3</v>
       </c>
       <c r="P139">
-        <v>902.87971044165306</v>
+        <v>593.26406686834218</v>
       </c>
       <c r="Q139">
-        <v>3.1989730845907623E-2</v>
+        <v>59.210682000870626</v>
       </c>
       <c r="R139">
-        <v>1.9348118221216299</v>
+        <v>1.7315505182804289</v>
       </c>
       <c r="S139">
-        <v>2.562033223463267E-4</v>
+        <v>4.8265890546990153E-2</v>
       </c>
       <c r="T139">
         <v>2.4576589400968962E+19</v>
@@ -15931,58 +15928,58 @@
         <v>143</v>
       </c>
       <c r="B140">
-        <v>29487</v>
+        <v>29493</v>
       </c>
       <c r="C140" t="s">
         <v>174</v>
       </c>
       <c r="D140">
-        <v>0.378</v>
+        <v>0.41899999999999998</v>
       </c>
       <c r="E140">
-        <v>-6.0000000000000053E-3</v>
+        <v>-1.0000000000000011E-3</v>
       </c>
       <c r="F140">
-        <v>7.0000000000000062E-3</v>
+        <v>5.0000000000000044E-4</v>
       </c>
       <c r="G140" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H140" t="s">
+        <v>196</v>
+      </c>
+      <c r="I140" t="s">
         <v>197</v>
       </c>
-      <c r="I140" t="s">
-        <v>198</v>
-      </c>
       <c r="J140">
-        <v>879670.00269436976</v>
+        <v>2209625.3528996678</v>
       </c>
       <c r="K140">
-        <v>81495.275520363808</v>
+        <v>78460.513956318231</v>
       </c>
       <c r="L140">
-        <v>-0.4387348172057895</v>
+        <v>-0.41663218755876291</v>
       </c>
       <c r="M140">
-        <v>2.1987985720624552E-3</v>
+        <v>2.3719691009227439E-5</v>
       </c>
       <c r="N140">
-        <v>-0.24798054885544629</v>
+        <v>-0.23548775818538781</v>
       </c>
       <c r="O140">
-        <v>1.2427991929048481E-3</v>
+        <v>1.340678187478073E-5</v>
       </c>
       <c r="P140">
-        <v>593.26406686834218</v>
+        <v>526.47063279562269</v>
       </c>
       <c r="Q140">
-        <v>59.210682000870626</v>
+        <v>7.0454066259993624</v>
       </c>
       <c r="R140">
-        <v>1.7315505182804289</v>
+        <v>1.7392511518129969</v>
       </c>
       <c r="S140">
-        <v>4.8265890546990153E-2</v>
+        <v>1.8733710035047531E-2</v>
       </c>
       <c r="T140">
         <v>2.9521970303271739E+19</v>
@@ -16056,52 +16053,52 @@
         <v>175</v>
       </c>
       <c r="D141">
-        <v>0.41899999999999998</v>
+        <v>0.4395</v>
       </c>
       <c r="E141">
-        <v>-1.0000000000000011E-3</v>
+        <v>-5.0000000000000044E-4</v>
       </c>
       <c r="F141">
-        <v>5.0000000000000044E-4</v>
+        <v>4.0000000000001151E-4</v>
       </c>
       <c r="G141" t="s">
         <v>191</v>
       </c>
       <c r="H141" t="s">
+        <v>196</v>
+      </c>
+      <c r="I141" t="s">
         <v>197</v>
       </c>
-      <c r="I141" t="s">
-        <v>198</v>
-      </c>
       <c r="J141">
-        <v>2209625.3528996678</v>
+        <v>2819747.6562088672</v>
       </c>
       <c r="K141">
-        <v>78460.513956318231</v>
+        <v>103484.203771648</v>
       </c>
       <c r="L141">
-        <v>-0.41663218755876291</v>
+        <v>-0.39895674020393451</v>
       </c>
       <c r="M141">
-        <v>2.3719691009227439E-5</v>
+        <v>1.2640136613976669E-3</v>
       </c>
       <c r="N141">
-        <v>-0.23548775818538781</v>
+        <v>-0.22549728794135429</v>
       </c>
       <c r="O141">
-        <v>1.340678187478073E-5</v>
+        <v>7.1444250426824785E-4</v>
       </c>
       <c r="P141">
-        <v>526.47063279562269</v>
+        <v>532.25522354842542</v>
       </c>
       <c r="Q141">
-        <v>7.0454066259993624</v>
+        <v>1.0064677032828511</v>
       </c>
       <c r="R141">
-        <v>1.7392511518129969</v>
+        <v>1.798617489558769</v>
       </c>
       <c r="S141">
-        <v>1.8733710035047531E-2</v>
+        <v>2.145790715971652E-3</v>
       </c>
       <c r="T141">
         <v>3.049002613797301E+19</v>
@@ -16169,58 +16166,58 @@
         <v>145</v>
       </c>
       <c r="B142">
-        <v>29493</v>
+        <v>29496</v>
       </c>
       <c r="C142" t="s">
         <v>176</v>
       </c>
       <c r="D142">
-        <v>0.4395</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="E142">
-        <v>-5.0000000000000044E-4</v>
+        <v>-1.0000000000000011E-3</v>
       </c>
       <c r="F142">
-        <v>4.0000000000001151E-4</v>
+        <v>1.0000000000000011E-3</v>
       </c>
       <c r="G142" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H142" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I142" t="s">
         <v>198</v>
       </c>
       <c r="J142">
-        <v>2819747.6562088672</v>
+        <v>3319325.986601959</v>
       </c>
       <c r="K142">
-        <v>103484.203771648</v>
+        <v>162962.7532923086</v>
       </c>
       <c r="L142">
-        <v>-0.39895674020393451</v>
+        <v>-0.42217533557199799</v>
       </c>
       <c r="M142">
-        <v>1.2640136613976669E-3</v>
+        <v>2.9089478578070432E-4</v>
       </c>
       <c r="N142">
-        <v>-0.22549728794135429</v>
+        <v>-0.2386208418450424</v>
       </c>
       <c r="O142">
-        <v>7.1444250426824785E-4</v>
+        <v>1.6441879196299469E-4</v>
       </c>
       <c r="P142">
-        <v>532.25522354842542</v>
+        <v>415.51941034503648</v>
       </c>
       <c r="Q142">
-        <v>1.0064677032828511</v>
+        <v>4.8768797868460751</v>
       </c>
       <c r="R142">
-        <v>1.798617489558769</v>
+        <v>1.5330718032171879</v>
       </c>
       <c r="S142">
-        <v>2.145790715971652E-3</v>
+        <v>7.730968218773171E-4</v>
       </c>
       <c r="T142">
         <v>3.1099949356188799E+19</v>
@@ -16294,7 +16291,7 @@
         <v>177</v>
       </c>
       <c r="D143">
-        <v>0.27900000000000003</v>
+        <v>0.66100000000000003</v>
       </c>
       <c r="E143">
         <v>-1.0000000000000011E-3</v>
@@ -16306,40 +16303,40 @@
         <v>191</v>
       </c>
       <c r="H143" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I143" t="s">
         <v>198</v>
       </c>
       <c r="J143">
-        <v>3319325.986601959</v>
+        <v>3035425.25</v>
       </c>
       <c r="K143">
-        <v>162962.7532923086</v>
+        <v>35123.270363335527</v>
       </c>
       <c r="L143">
-        <v>-0.42217533557199799</v>
+        <v>-0.38773426413536072</v>
       </c>
       <c r="M143">
-        <v>2.9089478578070432E-4</v>
+        <v>0</v>
       </c>
       <c r="N143">
-        <v>-0.2386208418450424</v>
+        <v>-0.21915414929389959</v>
       </c>
       <c r="O143">
-        <v>1.6441879196299469E-4</v>
+        <v>0</v>
       </c>
       <c r="P143">
-        <v>415.51941034503648</v>
+        <v>330.54685014101369</v>
       </c>
       <c r="Q143">
-        <v>4.8768797868460751</v>
+        <v>7.0720159311214266</v>
       </c>
       <c r="R143">
-        <v>1.5330718032171879</v>
+        <v>1.4232122898101811</v>
       </c>
       <c r="S143">
-        <v>7.730968218773171E-4</v>
+        <v>0</v>
       </c>
       <c r="T143">
         <v>2.384500413544235E+19</v>
@@ -16407,13 +16404,13 @@
         <v>147</v>
       </c>
       <c r="B144">
-        <v>29496</v>
+        <v>27571</v>
       </c>
       <c r="C144" t="s">
         <v>178</v>
       </c>
       <c r="D144">
-        <v>0.66100000000000003</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="E144">
         <v>-1.0000000000000011E-3</v>
@@ -16422,43 +16419,43 @@
         <v>1.0000000000000011E-3</v>
       </c>
       <c r="G144" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H144" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I144" t="s">
         <v>198</v>
       </c>
       <c r="J144">
-        <v>3035425.25</v>
+        <v>3750493.8205085951</v>
       </c>
       <c r="K144">
-        <v>35123.270363335527</v>
+        <v>50651.901238690873</v>
       </c>
       <c r="L144">
-        <v>-0.38773426413536072</v>
+        <v>-0.43331165823352003</v>
       </c>
       <c r="M144">
-        <v>0</v>
+        <v>1.3359678611448711E-3</v>
       </c>
       <c r="N144">
-        <v>-0.21915414929389959</v>
+        <v>-0.24491528508851129</v>
       </c>
       <c r="O144">
-        <v>0</v>
+        <v>7.5511226934277254E-4</v>
       </c>
       <c r="P144">
-        <v>330.54685014101369</v>
+        <v>744.95541280658711</v>
       </c>
       <c r="Q144">
-        <v>7.0720159311214266</v>
+        <v>2.281382397146785</v>
       </c>
       <c r="R144">
-        <v>1.4232122898101811</v>
+        <v>1.706069757181309</v>
       </c>
       <c r="S144">
-        <v>0</v>
+        <v>6.6765372052548511E-3</v>
       </c>
       <c r="T144">
         <v>6.1660243312072237E+19</v>
@@ -16532,52 +16529,52 @@
         <v>179</v>
       </c>
       <c r="D145">
-        <v>0.25800000000000001</v>
+        <v>0.30649999999999999</v>
       </c>
       <c r="E145">
-        <v>-1.0000000000000011E-3</v>
+        <v>-5.0000000000000044E-4</v>
       </c>
       <c r="F145">
-        <v>1.0000000000000011E-3</v>
+        <v>5.0000000000000044E-4</v>
       </c>
       <c r="G145" t="s">
         <v>191</v>
       </c>
       <c r="H145" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I145" t="s">
         <v>198</v>
       </c>
       <c r="J145">
-        <v>3750493.8205085951</v>
+        <v>4218690.906718879</v>
       </c>
       <c r="K145">
-        <v>50651.901238690873</v>
+        <v>222788.2276934252</v>
       </c>
       <c r="L145">
-        <v>-0.43331165823352003</v>
+        <v>-0.42838151621939619</v>
       </c>
       <c r="M145">
-        <v>1.3359678611448711E-3</v>
+        <v>1.7914550699759111E-3</v>
       </c>
       <c r="N145">
-        <v>-0.24491528508851129</v>
+        <v>-0.24212868308052829</v>
       </c>
       <c r="O145">
-        <v>7.5511226934277254E-4</v>
+        <v>1.0125615612907311E-3</v>
       </c>
       <c r="P145">
-        <v>744.95541280658711</v>
+        <v>720.59863046024304</v>
       </c>
       <c r="Q145">
-        <v>2.281382397146785</v>
+        <v>10.669854481732269</v>
       </c>
       <c r="R145">
-        <v>1.706069757181309</v>
+        <v>1.6781562279334661</v>
       </c>
       <c r="S145">
-        <v>6.6765372052548511E-3</v>
+        <v>1.226927020003377E-3</v>
       </c>
       <c r="T145">
         <v>3.0424896733965111E+19</v>
@@ -16645,58 +16642,58 @@
         <v>149</v>
       </c>
       <c r="B146">
-        <v>27571</v>
+        <v>27572</v>
       </c>
       <c r="C146" t="s">
         <v>180</v>
       </c>
       <c r="D146">
-        <v>0.30649999999999999</v>
+        <v>0.26</v>
       </c>
       <c r="E146">
-        <v>-5.0000000000000044E-4</v>
+        <v>-5.0000000000000036E-3</v>
       </c>
       <c r="F146">
-        <v>5.0000000000000044E-4</v>
+        <v>1.0000000000000011E-3</v>
       </c>
       <c r="G146" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H146" t="s">
+        <v>196</v>
+      </c>
+      <c r="I146" t="s">
         <v>197</v>
       </c>
-      <c r="I146" t="s">
-        <v>198</v>
-      </c>
       <c r="J146">
-        <v>4218690.906718879</v>
+        <v>3892352.6164442222</v>
       </c>
       <c r="K146">
-        <v>222788.2276934252</v>
+        <v>213174.20299351169</v>
       </c>
       <c r="L146">
-        <v>-0.42838151621939619</v>
+        <v>-0.43288490787376199</v>
       </c>
       <c r="M146">
-        <v>1.7914550699759111E-3</v>
+        <v>6.4052100380485033E-4</v>
       </c>
       <c r="N146">
-        <v>-0.24212868308052829</v>
+        <v>-0.24467407836343069</v>
       </c>
       <c r="O146">
-        <v>1.0125615612907311E-3</v>
+        <v>3.6203361084621849E-4</v>
       </c>
       <c r="P146">
-        <v>720.59863046024304</v>
+        <v>748.90437836384467</v>
       </c>
       <c r="Q146">
-        <v>10.669854481732269</v>
+        <v>5.075144073151364</v>
       </c>
       <c r="R146">
-        <v>1.6781562279334661</v>
+        <v>1.6870154616333819</v>
       </c>
       <c r="S146">
-        <v>1.226927020003377E-3</v>
+        <v>4.9688945336237023E-3</v>
       </c>
       <c r="T146">
         <v>3.682007880691714E+19</v>
@@ -16770,52 +16767,52 @@
         <v>181</v>
       </c>
       <c r="D147">
-        <v>0.26</v>
+        <v>0.27350000000000002</v>
       </c>
       <c r="E147">
-        <v>-5.0000000000000036E-3</v>
+        <v>-5.0000000000000044E-4</v>
       </c>
       <c r="F147">
-        <v>1.0000000000000011E-3</v>
+        <v>5.5000000000000049E-3</v>
       </c>
       <c r="G147" t="s">
         <v>191</v>
       </c>
       <c r="H147" t="s">
+        <v>196</v>
+      </c>
+      <c r="I147" t="s">
         <v>197</v>
       </c>
-      <c r="I147" t="s">
-        <v>198</v>
-      </c>
       <c r="J147">
-        <v>3892352.6164442222</v>
+        <v>4186991.7411835599</v>
       </c>
       <c r="K147">
-        <v>213174.20299351169</v>
+        <v>355501.13914165972</v>
       </c>
       <c r="L147">
-        <v>-0.43288490787376199</v>
+        <v>-0.43572490569966998</v>
       </c>
       <c r="M147">
-        <v>6.4052100380485033E-4</v>
+        <v>7.1986984016192412E-4</v>
       </c>
       <c r="N147">
-        <v>-0.24467407836343069</v>
+        <v>-0.2462792945259005</v>
       </c>
       <c r="O147">
-        <v>3.6203361084621849E-4</v>
+        <v>4.068829531349849E-4</v>
       </c>
       <c r="P147">
-        <v>748.90437836384467</v>
+        <v>750.32088594879031</v>
       </c>
       <c r="Q147">
-        <v>5.075144073151364</v>
+        <v>7.6037445213604542</v>
       </c>
       <c r="R147">
-        <v>1.6870154616333819</v>
+        <v>1.707746138037276</v>
       </c>
       <c r="S147">
-        <v>4.9688945336237023E-3</v>
+        <v>2.4395883763542289E-2</v>
       </c>
       <c r="T147">
         <v>2.269629059940268E+19</v>
@@ -16883,58 +16880,58 @@
         <v>151</v>
       </c>
       <c r="B148">
-        <v>27572</v>
+        <v>27573</v>
       </c>
       <c r="C148" t="s">
         <v>182</v>
       </c>
       <c r="D148">
-        <v>0.27350000000000002</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="E148">
-        <v>-5.0000000000000044E-4</v>
+        <v>-6.0000000000000053E-3</v>
       </c>
       <c r="F148">
-        <v>5.5000000000000049E-3</v>
+        <v>9.9999999999988987E-5</v>
       </c>
       <c r="G148" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H148" t="s">
+        <v>196</v>
+      </c>
+      <c r="I148" t="s">
         <v>197</v>
       </c>
-      <c r="I148" t="s">
-        <v>198</v>
-      </c>
       <c r="J148">
-        <v>4186991.7411835599</v>
+        <v>3941639.922015307</v>
       </c>
       <c r="K148">
-        <v>355501.13914165972</v>
+        <v>210303.83688353479</v>
       </c>
       <c r="L148">
-        <v>-0.43572490569966998</v>
+        <v>-0.43619160453035688</v>
       </c>
       <c r="M148">
-        <v>7.1986984016192412E-4</v>
+        <v>1.7846631592982609E-3</v>
       </c>
       <c r="N148">
-        <v>-0.2462792945259005</v>
+        <v>-0.24654308082150611</v>
       </c>
       <c r="O148">
-        <v>4.068829531349849E-4</v>
+        <v>1.008722655255534E-3</v>
       </c>
       <c r="P148">
-        <v>750.32088594879031</v>
+        <v>746.51092190759096</v>
       </c>
       <c r="Q148">
-        <v>7.6037445213604542</v>
+        <v>4.8876145666509956</v>
       </c>
       <c r="R148">
-        <v>1.707746138037276</v>
+        <v>1.694409348817455</v>
       </c>
       <c r="S148">
-        <v>2.4395883763542289E-2</v>
+        <v>8.9756262472964199E-3</v>
       </c>
       <c r="T148">
         <v>2.2807122894747202E+19</v>
@@ -17008,52 +17005,52 @@
         <v>183</v>
       </c>
       <c r="D149">
-        <v>0.26800000000000002</v>
+        <v>0.27510000000000001</v>
       </c>
       <c r="E149">
-        <v>-6.0000000000000053E-3</v>
+        <v>-9.9999999999988987E-5</v>
       </c>
       <c r="F149">
-        <v>9.9999999999988987E-5</v>
+        <v>4.0000000000001151E-4</v>
       </c>
       <c r="G149" t="s">
         <v>191</v>
       </c>
       <c r="H149" t="s">
+        <v>196</v>
+      </c>
+      <c r="I149" t="s">
         <v>197</v>
       </c>
-      <c r="I149" t="s">
-        <v>198</v>
-      </c>
       <c r="J149">
-        <v>3941639.922015307</v>
+        <v>4715452.4559823023</v>
       </c>
       <c r="K149">
-        <v>210303.83688353479</v>
+        <v>163508.88873886509</v>
       </c>
       <c r="L149">
-        <v>-0.43619160453035688</v>
+        <v>-0.43796136982633221</v>
       </c>
       <c r="M149">
-        <v>1.7846631592982609E-3</v>
+        <v>5.7073057435574892E-5</v>
       </c>
       <c r="N149">
-        <v>-0.24654308082150611</v>
+        <v>-0.24754338294531819</v>
       </c>
       <c r="O149">
-        <v>1.008722655255534E-3</v>
+        <v>3.2258684637492818E-5</v>
       </c>
       <c r="P149">
-        <v>746.51092190759096</v>
+        <v>747.82766918532127</v>
       </c>
       <c r="Q149">
-        <v>4.8876145666509956</v>
+        <v>2.982617140941215</v>
       </c>
       <c r="R149">
-        <v>1.694409348817455</v>
+        <v>1.6988010245156779</v>
       </c>
       <c r="S149">
-        <v>8.9756262472964199E-3</v>
+        <v>3.2993559958647278E-3</v>
       </c>
       <c r="T149">
         <v>1.8547148062704091E+19</v>
@@ -17121,58 +17118,58 @@
         <v>153</v>
       </c>
       <c r="B150">
-        <v>27573</v>
+        <v>27587</v>
       </c>
       <c r="C150" t="s">
         <v>184</v>
       </c>
       <c r="D150">
-        <v>0.27510000000000001</v>
+        <v>0.222</v>
       </c>
       <c r="E150">
-        <v>-9.9999999999988987E-5</v>
+        <v>-1.0000000000000011E-3</v>
       </c>
       <c r="F150">
-        <v>4.0000000000001151E-4</v>
+        <v>1.0000000000000011E-3</v>
       </c>
       <c r="G150" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H150" t="s">
+        <v>196</v>
+      </c>
+      <c r="I150" t="s">
         <v>197</v>
       </c>
-      <c r="I150" t="s">
-        <v>198</v>
-      </c>
       <c r="J150">
-        <v>4715452.4559823023</v>
+        <v>4588596.4815972392</v>
       </c>
       <c r="K150">
-        <v>163508.88873886509</v>
+        <v>238411.11357826411</v>
       </c>
       <c r="L150">
-        <v>-0.43796136982633221</v>
+        <v>-0.43201898251760218</v>
       </c>
       <c r="M150">
-        <v>5.7073057435574892E-5</v>
+        <v>5.4622940657556018E-4</v>
       </c>
       <c r="N150">
-        <v>-0.24754338294531819</v>
+        <v>-0.24418464229255779</v>
       </c>
       <c r="O150">
-        <v>3.2258684637492818E-5</v>
+        <v>3.0873836023836981E-4</v>
       </c>
       <c r="P150">
-        <v>747.82766918532127</v>
+        <v>736.57632038757538</v>
       </c>
       <c r="Q150">
-        <v>2.982617140941215</v>
+        <v>5.8793014534968506</v>
       </c>
       <c r="R150">
-        <v>1.6988010245156779</v>
+        <v>1.601949021022963</v>
       </c>
       <c r="S150">
-        <v>3.2993559958647278E-3</v>
+        <v>2.0503540519274388E-3</v>
       </c>
       <c r="T150">
         <v>1.9741093453535068E+19</v>
@@ -17246,7 +17243,7 @@
         <v>185</v>
       </c>
       <c r="D151">
-        <v>0.222</v>
+        <v>0.26800000000000002</v>
       </c>
       <c r="E151">
         <v>-1.0000000000000011E-3</v>
@@ -17258,40 +17255,40 @@
         <v>191</v>
       </c>
       <c r="H151" t="s">
+        <v>196</v>
+      </c>
+      <c r="I151" t="s">
         <v>197</v>
       </c>
-      <c r="I151" t="s">
-        <v>198</v>
-      </c>
       <c r="J151">
-        <v>4588596.4815972392</v>
+        <v>4236403.2069686009</v>
       </c>
       <c r="K151">
-        <v>238411.11357826411</v>
+        <v>129089.8988809162</v>
       </c>
       <c r="L151">
-        <v>-0.43201898251760218</v>
+        <v>-0.43937213863600699</v>
       </c>
       <c r="M151">
-        <v>5.4622940657556018E-4</v>
+        <v>1.7862336981144811E-4</v>
       </c>
       <c r="N151">
-        <v>-0.24418464229255779</v>
+        <v>-0.24834077401165619</v>
       </c>
       <c r="O151">
-        <v>3.0873836023836981E-4</v>
+        <v>1.009610351108137E-4</v>
       </c>
       <c r="P151">
-        <v>736.57632038757538</v>
+        <v>746.88192045496862</v>
       </c>
       <c r="Q151">
-        <v>5.8793014534968506</v>
+        <v>4.5330715430068267</v>
       </c>
       <c r="R151">
-        <v>1.601949021022963</v>
+        <v>1.701276071259856</v>
       </c>
       <c r="S151">
-        <v>2.0503540519274388E-3</v>
+        <v>1.922513887895327E-3</v>
       </c>
       <c r="T151">
         <v>1.7768139258449209E+19</v>
@@ -17359,58 +17356,58 @@
         <v>155</v>
       </c>
       <c r="B152">
-        <v>27587</v>
+        <v>27588</v>
       </c>
       <c r="C152" t="s">
         <v>186</v>
       </c>
       <c r="D152">
-        <v>0.26800000000000002</v>
+        <v>0.22220000000000001</v>
       </c>
       <c r="E152">
-        <v>-1.0000000000000011E-3</v>
+        <v>-2.000000000000057E-4</v>
       </c>
       <c r="F152">
-        <v>1.0000000000000011E-3</v>
+        <v>9.9999999999988987E-5</v>
       </c>
       <c r="G152" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H152" t="s">
+        <v>196</v>
+      </c>
+      <c r="I152" t="s">
         <v>197</v>
       </c>
-      <c r="I152" t="s">
-        <v>198</v>
-      </c>
       <c r="J152">
-        <v>4236403.2069686009</v>
+        <v>4391535.1043176688</v>
       </c>
       <c r="K152">
-        <v>129089.8988809162</v>
+        <v>103103.88782239291</v>
       </c>
       <c r="L152">
-        <v>-0.43937213863600699</v>
+        <v>-0.43300750837020968</v>
       </c>
       <c r="M152">
-        <v>1.7862336981144811E-4</v>
+        <v>1.332165081185943E-5</v>
       </c>
       <c r="N152">
-        <v>-0.24834077401165619</v>
+        <v>-0.24474337429620549</v>
       </c>
       <c r="O152">
-        <v>1.009610351108137E-4</v>
+        <v>7.5296287197490494E-6</v>
       </c>
       <c r="P152">
-        <v>746.88192045496862</v>
+        <v>738.7927494305909</v>
       </c>
       <c r="Q152">
-        <v>4.5330715430068267</v>
+        <v>2.6130805381219488</v>
       </c>
       <c r="R152">
-        <v>1.701276071259856</v>
+        <v>1.605794141644274</v>
       </c>
       <c r="S152">
-        <v>1.922513887895327E-3</v>
+        <v>1.8532293827333571E-4</v>
       </c>
       <c r="T152">
         <v>1.6851080753740249E+19</v>
@@ -17484,52 +17481,52 @@
         <v>187</v>
       </c>
       <c r="D153">
-        <v>0.22220000000000001</v>
+        <v>0.26669999999999999</v>
       </c>
       <c r="E153">
-        <v>-2.000000000000057E-4</v>
+        <v>-1.6999999999999791E-3</v>
       </c>
       <c r="F153">
-        <v>9.9999999999988987E-5</v>
+        <v>3.0000000000002253E-4</v>
       </c>
       <c r="G153" t="s">
         <v>191</v>
       </c>
       <c r="H153" t="s">
+        <v>196</v>
+      </c>
+      <c r="I153" t="s">
         <v>197</v>
       </c>
-      <c r="I153" t="s">
-        <v>198</v>
-      </c>
       <c r="J153">
-        <v>4391535.1043176688</v>
+        <v>4353191.2735415008</v>
       </c>
       <c r="K153">
-        <v>103103.88782239291</v>
+        <v>174631.46241266999</v>
       </c>
       <c r="L153">
-        <v>-0.43300750837020968</v>
+        <v>-0.43920220227181261</v>
       </c>
       <c r="M153">
-        <v>1.332165081185943E-5</v>
+        <v>1.857044083637405E-4</v>
       </c>
       <c r="N153">
-        <v>-0.24474337429620549</v>
+        <v>-0.2482447230231985</v>
       </c>
       <c r="O153">
-        <v>7.5296287197490494E-6</v>
+        <v>1.0496336124907189E-4</v>
       </c>
       <c r="P153">
-        <v>738.7927494305909</v>
+        <v>749.5021428162712</v>
       </c>
       <c r="Q153">
-        <v>2.6130805381219488</v>
+        <v>2.9901964862131081</v>
       </c>
       <c r="R153">
-        <v>1.605794141644274</v>
+        <v>1.700067442004896</v>
       </c>
       <c r="S153">
-        <v>1.8532293827333571E-4</v>
+        <v>8.6146436830936146E-3</v>
       </c>
       <c r="T153">
         <v>1.6123800750222209E+19</v>
@@ -17597,58 +17594,58 @@
         <v>157</v>
       </c>
       <c r="B154">
-        <v>27588</v>
+        <v>27589</v>
       </c>
       <c r="C154" t="s">
         <v>188</v>
       </c>
       <c r="D154">
-        <v>0.26669999999999999</v>
+        <v>0.2001</v>
       </c>
       <c r="E154">
-        <v>-1.6999999999999791E-3</v>
+        <v>-9.9999999999988987E-5</v>
       </c>
       <c r="F154">
-        <v>3.0000000000002253E-4</v>
+        <v>9.000000000000119E-4</v>
       </c>
       <c r="G154" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H154" t="s">
+        <v>196</v>
+      </c>
+      <c r="I154" t="s">
         <v>197</v>
       </c>
-      <c r="I154" t="s">
-        <v>198</v>
-      </c>
       <c r="J154">
-        <v>4353191.2735415008</v>
+        <v>2714063.6690177289</v>
       </c>
       <c r="K154">
-        <v>174631.46241266999</v>
+        <v>49074.788499381742</v>
       </c>
       <c r="L154">
-        <v>-0.43920220227181261</v>
+        <v>-0.42399052656886288</v>
       </c>
       <c r="M154">
-        <v>1.857044083637405E-4</v>
+        <v>2.8585733657182638E-4</v>
       </c>
       <c r="N154">
-        <v>-0.2482447230231985</v>
+        <v>-0.23964681936500951</v>
       </c>
       <c r="O154">
-        <v>1.0496336124907189E-4</v>
+        <v>1.615715380623439E-4</v>
       </c>
       <c r="P154">
-        <v>749.5021428162712</v>
+        <v>732.84862199841041</v>
       </c>
       <c r="Q154">
-        <v>2.9901964862131081</v>
+        <v>0.83961642709289208</v>
       </c>
       <c r="R154">
-        <v>1.700067442004896</v>
+        <v>1.810351134648039</v>
       </c>
       <c r="S154">
-        <v>8.6146436830936146E-3</v>
+        <v>1.1079169708980929E-2</v>
       </c>
       <c r="T154">
         <v>1.4361366076070629E+19</v>
@@ -17722,52 +17719,52 @@
         <v>189</v>
       </c>
       <c r="D155">
-        <v>0.2001</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="E155">
-        <v>-9.9999999999988987E-5</v>
+        <v>-1.0000000000000011E-3</v>
       </c>
       <c r="F155">
-        <v>9.000000000000119E-4</v>
+        <v>2.9999999999996701E-4</v>
       </c>
       <c r="G155" t="s">
         <v>191</v>
       </c>
       <c r="H155" t="s">
+        <v>196</v>
+      </c>
+      <c r="I155" t="s">
         <v>197</v>
       </c>
-      <c r="I155" t="s">
-        <v>198</v>
-      </c>
       <c r="J155">
-        <v>2714063.6690177289</v>
+        <v>4369409.876333599</v>
       </c>
       <c r="K155">
-        <v>49074.788499381742</v>
+        <v>316260.67861246457</v>
       </c>
       <c r="L155">
-        <v>-0.42399052656886288</v>
+        <v>-0.42383559770812962</v>
       </c>
       <c r="M155">
-        <v>2.8585733657182638E-4</v>
+        <v>2.8129163388407319E-3</v>
       </c>
       <c r="N155">
-        <v>-0.23964681936500951</v>
+        <v>-0.2395592508785081</v>
       </c>
       <c r="O155">
-        <v>1.615715380623439E-4</v>
+        <v>1.589909234996939E-3</v>
       </c>
       <c r="P155">
-        <v>732.84862199841041</v>
+        <v>732.82613939934993</v>
       </c>
       <c r="Q155">
-        <v>0.83961642709289208</v>
+        <v>2.7055113256108139</v>
       </c>
       <c r="R155">
-        <v>1.810351134648039</v>
+        <v>1.667788140954229</v>
       </c>
       <c r="S155">
-        <v>1.1079169708980929E-2</v>
+        <v>1.3936962067566669E-3</v>
       </c>
       <c r="T155">
         <v>2.7908409821731402E+19</v>
@@ -17828,125 +17825,6 @@
       </c>
       <c r="AM155">
         <v>0.1163866002781084</v>
-      </c>
-    </row>
-    <row r="156" spans="1:39" x14ac:dyDescent="0.45">
-      <c r="A156" s="1">
-        <v>159</v>
-      </c>
-      <c r="B156">
-        <v>27589</v>
-      </c>
-      <c r="C156" t="s">
-        <v>190</v>
-      </c>
-      <c r="D156">
-        <v>0.32900000000000001</v>
-      </c>
-      <c r="E156">
-        <v>-1.0000000000000011E-3</v>
-      </c>
-      <c r="F156">
-        <v>2.9999999999996701E-4</v>
-      </c>
-      <c r="G156" t="s">
-        <v>192</v>
-      </c>
-      <c r="H156" t="s">
-        <v>197</v>
-      </c>
-      <c r="I156" t="s">
-        <v>198</v>
-      </c>
-      <c r="J156">
-        <v>4369409.876333599</v>
-      </c>
-      <c r="K156">
-        <v>316260.67861246457</v>
-      </c>
-      <c r="L156">
-        <v>-0.42383559770812962</v>
-      </c>
-      <c r="M156">
-        <v>2.8129163388407319E-3</v>
-      </c>
-      <c r="N156">
-        <v>-0.2395592508785081</v>
-      </c>
-      <c r="O156">
-        <v>1.589909234996939E-3</v>
-      </c>
-      <c r="P156">
-        <v>732.82613939934993</v>
-      </c>
-      <c r="Q156">
-        <v>2.7055113256108139</v>
-      </c>
-      <c r="R156">
-        <v>1.667788140954229</v>
-      </c>
-      <c r="S156">
-        <v>1.3936962067566669E-3</v>
-      </c>
-      <c r="T156">
-        <v>2.2631680069179011E+19</v>
-      </c>
-      <c r="U156">
-        <v>3.2451279854387738E+18</v>
-      </c>
-      <c r="V156">
-        <v>1.140825558604782E+19</v>
-      </c>
-      <c r="W156">
-        <v>6.1046903778540728E+18</v>
-      </c>
-      <c r="X156">
-        <v>2.589635379234062E+20</v>
-      </c>
-      <c r="Y156">
-        <v>5.7898774847853363E+18</v>
-      </c>
-      <c r="Z156">
-        <v>143.91782548539661</v>
-      </c>
-      <c r="AA156">
-        <v>301.3640949363064</v>
-      </c>
-      <c r="AB156">
-        <v>774.27952015387416</v>
-      </c>
-      <c r="AC156">
-        <v>3376.6187064854712</v>
-      </c>
-      <c r="AD156">
-        <v>948.40537588680036</v>
-      </c>
-      <c r="AE156">
-        <v>286.11829148071581</v>
-      </c>
-      <c r="AF156">
-        <v>920.29274859930752</v>
-      </c>
-      <c r="AG156">
-        <v>3538.3774121044371</v>
-      </c>
-      <c r="AH156">
-        <v>0.51257232504731376</v>
-      </c>
-      <c r="AI156">
-        <v>1.048573063443081E-3</v>
-      </c>
-      <c r="AJ156">
-        <v>0.50949627036057898</v>
-      </c>
-      <c r="AK156">
-        <v>1.0880909806163519E-3</v>
-      </c>
-      <c r="AL156">
-        <v>25.01116973559412</v>
-      </c>
-      <c r="AM156">
-        <v>0.1011108218296215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>